<commit_message>
#14 adding more sophisticated implementation of a merged cell matcher. Cell contents aren't used just the cell addresses within the region. Renamed the count based matcher for clarity.
</commit_message>
<xml_diff>
--- a/src/test/resource/bad/robot/excel/mergedRegionSheet.xlsx
+++ b/src/test/resource/bad/robot/excel/mergedRegionSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toby/code/github/simple-excel/src/test/resource/bad/robot/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559E957F-287C-A845-9E58-4A50C58592FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E548C4-FC15-694F-8F57-124C17F5BE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="19440" windowHeight="10040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -648,7 +648,7 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>